<commit_message>
Update Clash of Cosplayers - Plan Outline.xlsx
</commit_message>
<xml_diff>
--- a/Shared Documentation/Luke's Documents/Clash of Cosplayers - Plan Outline.xlsx
+++ b/Shared Documentation/Luke's Documents/Clash of Cosplayers - Plan Outline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C2240950\Documents\GitHub\Project_Clash-of-Cosplayers\Shared Documentation\Luke's Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0158F4B-14DB-4689-AFC1-7CC3A99F723F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1CF2E7-6D71-4B7C-A3CD-C290A785C62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{E57F7292-3F36-47CF-B64B-390F0A8E2C94}"/>
   </bookViews>
@@ -768,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BD4154-D683-48E3-B727-AD028CFBFA14}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>